<commit_message>
Making a commit before a possible mess up with remove pallet.
</commit_message>
<xml_diff>
--- a/apps/inertiion-services/data/Book1.xlsx
+++ b/apps/inertiion-services/data/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ozahn\Documents\source\scratchworks\apps\inertiion-services\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1CE61A-8473-4CF9-821B-17F4C6D810D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D189A55-E1D3-46E4-B2D7-13D6714FAFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6BEE52B8-C285-48F0-89A2-099468F840A7}"/>
+    <workbookView xWindow="4710" yWindow="75" windowWidth="19200" windowHeight="20910" xr2:uid="{6BEE52B8-C285-48F0-89A2-099468F840A7}"/>
   </bookViews>
   <sheets>
     <sheet name="mario" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>18-2-3</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>12-2-9</t>
+  </si>
+  <si>
+    <t>1A-3-1</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,41 +497,26 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>12</v>
       </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
       <c r="D4">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
@@ -542,13 +530,13 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>150</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>9</v>
@@ -559,16 +547,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>12</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>150</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
@@ -582,18 +570,38 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D7">
-        <v>23</v>
+        <v>150</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>150</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Some things are working as intended.
</commit_message>
<xml_diff>
--- a/apps/inertiion-services/data/Book1.xlsx
+++ b/apps/inertiion-services/data/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ozahn\Documents\source\scratchworks\apps\inertiion-services\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9930B90E-8CBB-4073-9115-C5AD41BBFA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE84EE8-82FC-4448-A096-D925014A4543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4710" yWindow="75" windowWidth="19200" windowHeight="20910" xr2:uid="{6BEE52B8-C285-48F0-89A2-099468F840A7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="136">
   <si>
     <t>Date</t>
   </si>
@@ -444,9 +444,6 @@
   </si>
   <si>
     <t>MAROON/NAVY/WHITE/CHARCOAL</t>
-  </si>
-  <si>
-    <t>01-4-3</t>
   </si>
 </sst>
 </file>
@@ -816,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25369458-18D2-4A91-9449-7F3542433993}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,11 +1654,6 @@
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>